<commit_message>
Changed the data based on cycle servers
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -250,19 +250,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.11695340000000001</c:v>
+                  <c:v>4.0532599999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1180488</c:v>
+                  <c:v>4.5536E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.14378280000000002</c:v>
+                  <c:v>5.0608200000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1479096</c:v>
+                  <c:v>5.2423399999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14169020000000002</c:v>
+                  <c:v>5.7444799999999997E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -338,19 +338,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8.7098199999999987E-2</c:v>
+                  <c:v>4.0937000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.1493600000000004E-2</c:v>
+                  <c:v>4.3787200000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11411579999999999</c:v>
+                  <c:v>4.4896999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11691119999999999</c:v>
+                  <c:v>4.2803800000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1199784</c:v>
+                  <c:v>4.4049999999999992E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -382,7 +382,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -390,13 +389,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1611622272"/>
-        <c:axId val="1611624992"/>
+        <c:axId val="660341712"/>
+        <c:axId val="660342256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1611622272"/>
+        <c:axId val="660341712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="3.0000000000000006E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -507,12 +507,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1611624992"/>
+        <c:crossAx val="660342256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1611624992"/>
+        <c:axId val="660342256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,7 +625,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1611622272"/>
+        <c:crossAx val="660341712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1266,16 +1266,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>500062</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1209675</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>347662</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1562,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,11 +1593,11 @@
       </c>
       <c r="B2">
         <f>AVERAGE(B12:B16)</f>
-        <v>0.11695340000000001</v>
+        <v>4.0532599999999995E-2</v>
       </c>
       <c r="C2">
         <f>AVERAGE(B20:B24)</f>
-        <v>8.7098199999999987E-2</v>
+        <v>4.0937000000000001E-2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1606,11 +1606,11 @@
       </c>
       <c r="B3">
         <f>AVERAGE(C12:C16)</f>
-        <v>0.1180488</v>
+        <v>4.5536E-2</v>
       </c>
       <c r="C3">
         <f>AVERAGE(C20:C24)</f>
-        <v>7.1493600000000004E-2</v>
+        <v>4.3787200000000005E-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1619,11 +1619,11 @@
       </c>
       <c r="B4">
         <f>AVERAGE(D12:D16)</f>
-        <v>0.14378280000000002</v>
+        <v>5.0608200000000006E-2</v>
       </c>
       <c r="C4">
         <f>AVERAGE(D20:D24)</f>
-        <v>0.11411579999999999</v>
+        <v>4.4896999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1632,11 +1632,11 @@
       </c>
       <c r="B5">
         <f>AVERAGE(E12:E16)</f>
-        <v>0.1479096</v>
+        <v>5.2423399999999995E-2</v>
       </c>
       <c r="C5">
         <f>AVERAGE(E20:E24)</f>
-        <v>0.11691119999999999</v>
+        <v>4.2803800000000003E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1645,11 +1645,16 @@
       </c>
       <c r="B6">
         <f>AVERAGE(F12:F16)</f>
-        <v>0.14169020000000002</v>
+        <v>5.7444799999999997E-2</v>
       </c>
       <c r="C6">
         <f>AVERAGE(F20:F24)</f>
-        <v>0.1199784</v>
+        <v>4.4049999999999992E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>4.1454999999999999E-2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1682,19 +1687,19 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <v>0.13725300000000001</v>
+        <v>4.1991000000000001E-2</v>
       </c>
       <c r="C12">
-        <v>0.15845699999999999</v>
+        <v>4.6531999999999997E-2</v>
       </c>
       <c r="D12">
-        <v>0.17322799999999999</v>
+        <v>5.2331999999999997E-2</v>
       </c>
       <c r="E12">
-        <v>0.146421</v>
+        <v>5.2831000000000003E-2</v>
       </c>
       <c r="F12">
-        <v>0.13927500000000001</v>
+        <v>5.7761E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1702,19 +1707,19 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <v>0.13980699999999999</v>
+        <v>4.1454999999999999E-2</v>
       </c>
       <c r="C13">
-        <v>0.102025</v>
+        <v>4.5295000000000002E-2</v>
       </c>
       <c r="D13">
-        <v>0.12753999999999999</v>
+        <v>5.1380000000000002E-2</v>
       </c>
       <c r="E13">
-        <v>0.18535499999999999</v>
+        <v>5.2145999999999998E-2</v>
       </c>
       <c r="F13">
-        <v>0.14061000000000001</v>
+        <v>5.7500000000000002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1722,19 +1727,19 @@
         <v>3</v>
       </c>
       <c r="B14">
-        <v>0.102038</v>
+        <v>3.9761999999999999E-2</v>
       </c>
       <c r="C14">
-        <v>0.128056</v>
+        <v>4.5268999999999997E-2</v>
       </c>
       <c r="D14">
-        <v>0.12694</v>
+        <v>5.1407000000000001E-2</v>
       </c>
       <c r="E14">
-        <v>0.14286599999999999</v>
+        <v>5.2857000000000001E-2</v>
       </c>
       <c r="F14">
-        <v>0.15337500000000001</v>
+        <v>5.7230000000000003E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1742,19 +1747,19 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <v>6.9843000000000002E-2</v>
+        <v>3.9723000000000001E-2</v>
       </c>
       <c r="C15">
-        <v>0.139103</v>
+        <v>4.5349E-2</v>
       </c>
       <c r="D15">
-        <v>0.16439799999999999</v>
+        <v>5.1406E-2</v>
       </c>
       <c r="E15">
-        <v>0.15009600000000001</v>
+        <v>5.2152999999999998E-2</v>
       </c>
       <c r="F15">
-        <v>0.14302200000000001</v>
+        <v>5.7361000000000002E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1762,19 +1767,19 @@
         <v>5</v>
       </c>
       <c r="B16">
-        <v>0.135826</v>
+        <v>3.9732000000000003E-2</v>
       </c>
       <c r="C16">
-        <v>6.2603000000000006E-2</v>
+        <v>4.5234999999999997E-2</v>
       </c>
       <c r="D16">
-        <v>0.126808</v>
+        <v>4.6516000000000002E-2</v>
       </c>
       <c r="E16">
-        <v>0.11481</v>
+        <v>5.2130000000000003E-2</v>
       </c>
       <c r="F16">
-        <v>0.13216900000000001</v>
+        <v>5.7371999999999999E-2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1807,19 +1812,19 @@
         <v>1</v>
       </c>
       <c r="B20">
-        <v>9.7626000000000004E-2</v>
+        <v>4.0697999999999998E-2</v>
       </c>
       <c r="C20">
-        <v>7.8982999999999998E-2</v>
+        <v>4.3825999999999997E-2</v>
       </c>
       <c r="D20">
-        <v>0.116046</v>
+        <v>4.6406999999999997E-2</v>
       </c>
       <c r="E20">
-        <v>0.113855</v>
+        <v>4.2811000000000002E-2</v>
       </c>
       <c r="F20">
-        <v>0.132385</v>
+        <v>4.3976000000000001E-2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1827,19 +1832,19 @@
         <v>2</v>
       </c>
       <c r="B21">
-        <v>0.11014400000000001</v>
+        <v>4.1008000000000003E-2</v>
       </c>
       <c r="C21">
-        <v>0.102614</v>
+        <v>4.3801E-2</v>
       </c>
       <c r="D21">
-        <v>0.102688</v>
+        <v>4.623E-2</v>
       </c>
       <c r="E21">
-        <v>0.14998700000000001</v>
+        <v>4.2819000000000003E-2</v>
       </c>
       <c r="F21">
-        <v>0.118217</v>
+        <v>4.4054000000000003E-2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1847,19 +1852,19 @@
         <v>3</v>
       </c>
       <c r="B22">
-        <v>6.1145999999999999E-2</v>
+        <v>4.0988999999999998E-2</v>
       </c>
       <c r="C22">
-        <v>6.4558000000000004E-2</v>
+        <v>4.3820999999999999E-2</v>
       </c>
       <c r="D22">
-        <v>0.117448</v>
+        <v>4.6224000000000001E-2</v>
       </c>
       <c r="E22">
-        <v>0.109419</v>
+        <v>4.2758999999999998E-2</v>
       </c>
       <c r="F22">
-        <v>0.113538</v>
+        <v>4.3945999999999999E-2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1867,19 +1872,19 @@
         <v>4</v>
       </c>
       <c r="B23">
-        <v>0.10387299999999999</v>
+        <v>4.1005E-2</v>
       </c>
       <c r="C23">
-        <v>3.6339000000000003E-2</v>
+        <v>4.3778999999999998E-2</v>
       </c>
       <c r="D23">
-        <v>0.11763899999999999</v>
+        <v>4.4363E-2</v>
       </c>
       <c r="E23">
-        <v>9.9464999999999998E-2</v>
+        <v>4.2826999999999997E-2</v>
       </c>
       <c r="F23">
-        <v>0.117169</v>
+        <v>4.4006000000000003E-2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1887,19 +1892,19 @@
         <v>5</v>
       </c>
       <c r="B24">
-        <v>6.2701999999999994E-2</v>
+        <v>4.0985000000000001E-2</v>
       </c>
       <c r="C24">
-        <v>7.4973999999999999E-2</v>
+        <v>4.3708999999999998E-2</v>
       </c>
       <c r="D24">
-        <v>0.116758</v>
+        <v>4.1260999999999999E-2</v>
       </c>
       <c r="E24">
-        <v>0.11183</v>
+        <v>4.2803000000000001E-2</v>
       </c>
       <c r="F24">
-        <v>0.11858299999999999</v>
+        <v>4.4268000000000002E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>